<commit_message>
Fix link to node 27
</commit_message>
<xml_diff>
--- a/noditos.xlsx
+++ b/noditos.xlsx
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BJ60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T14" workbookViewId="0">
-      <selection activeCell="BH9" sqref="BH9"/>
+    <sheetView tabSelected="1" topLeftCell="J39" workbookViewId="0">
+      <selection activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="BJ7" s="20">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:62" x14ac:dyDescent="0.25">
@@ -7130,7 +7130,7 @@
       </c>
       <c r="AM30" s="20">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="20">
         <f t="shared" si="32"/>
@@ -7707,7 +7707,7 @@
         <v>136</v>
       </c>
       <c r="AG37" s="3">
-        <v>81</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="6:61" x14ac:dyDescent="0.25">
@@ -9616,7 +9616,7 @@
         <v>119</v>
       </c>
       <c r="J60" s="3">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="K60" s="3">
         <v>98</v>

</xml_diff>